<commit_message>
Updated DST data for 2024
</commit_message>
<xml_diff>
--- a/input/dst/DKSTAT.xlsx
+++ b/input/dst/DKSTAT.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="288">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="289">
   <x:si>
     <x:t>Personer, der har fået dansk statsborgerskab efter tidligere statsborgerskab og tid</x:t>
   </x:si>
@@ -155,6 +155,9 @@
   </x:si>
   <x:si>
     <x:t>2023</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024</x:t>
   </x:si>
   <x:si>
     <x:t>Albanien</x:t>
@@ -1287,27 +1290,27 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:AT245"/>
+  <x:dimension ref="A1:AU245"/>
   <x:sheetViews>
     <x:sheetView tabSelected="0" workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
     <x:col min="1" max="1" width="40.710625" style="0" customWidth="1"/>
-    <x:col min="2" max="46" width="6.980625" style="0" customWidth="1"/>
+    <x:col min="2" max="47" width="6.980625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:46">
+    <x:row r="1" spans="1:47">
       <x:c r="A1" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:46">
+    <x:row r="2" spans="1:47">
       <x:c r="A2" s="2" t="s">
         <x:v>1</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:46">
+    <x:row r="3" spans="1:47">
       <x:c r="B3" s="3" t="s">
         <x:v>2</x:v>
       </x:c>
@@ -1443,10 +1446,13 @@
       <x:c r="AT3" s="3" t="s">
         <x:v>46</x:v>
       </x:c>
+      <x:c r="AU3" s="3" t="s">
+        <x:v>47</x:v>
+      </x:c>
     </x:row>
-    <x:row r="4" spans="1:46">
+    <x:row r="4" spans="1:47">
       <x:c r="A4" s="3" t="s">
-        <x:v>47</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="B4" s="4" t="n">
         <x:v>0</x:v>
@@ -1583,10 +1589,13 @@
       <x:c r="AT4" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU4" s="4" t="n">
+        <x:v>7</x:v>
+      </x:c>
     </x:row>
-    <x:row r="5" spans="1:46">
+    <x:row r="5" spans="1:47">
       <x:c r="A5" s="3" t="s">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="B5" s="4" t="n">
         <x:v>0</x:v>
@@ -1723,10 +1732,13 @@
       <x:c r="AT5" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU5" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="6" spans="1:46">
+    <x:row r="6" spans="1:47">
       <x:c r="A6" s="3" t="s">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="B6" s="4" t="n">
         <x:v>0</x:v>
@@ -1863,10 +1875,13 @@
       <x:c r="AT6" s="4" t="n">
         <x:v>13</x:v>
       </x:c>
+      <x:c r="AU6" s="4" t="n">
+        <x:v>25</x:v>
+      </x:c>
     </x:row>
-    <x:row r="7" spans="1:46">
+    <x:row r="7" spans="1:47">
       <x:c r="A7" s="3" t="s">
-        <x:v>50</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="B7" s="4" t="n">
         <x:v>7</x:v>
@@ -2003,10 +2018,13 @@
       <x:c r="AT7" s="4" t="n">
         <x:v>6</x:v>
       </x:c>
+      <x:c r="AU7" s="4" t="n">
+        <x:v>14</x:v>
+      </x:c>
     </x:row>
-    <x:row r="8" spans="1:46">
+    <x:row r="8" spans="1:47">
       <x:c r="A8" s="3" t="s">
-        <x:v>51</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="B8" s="4" t="n">
         <x:v>0</x:v>
@@ -2143,10 +2161,13 @@
       <x:c r="AT8" s="4" t="n">
         <x:v>46</x:v>
       </x:c>
+      <x:c r="AU8" s="4" t="n">
+        <x:v>118</x:v>
+      </x:c>
     </x:row>
-    <x:row r="9" spans="1:46">
+    <x:row r="9" spans="1:47">
       <x:c r="A9" s="3" t="s">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="B9" s="4" t="n">
         <x:v>12</x:v>
@@ -2283,10 +2304,13 @@
       <x:c r="AT9" s="4" t="n">
         <x:v>58</x:v>
       </x:c>
+      <x:c r="AU9" s="4" t="n">
+        <x:v>96</x:v>
+      </x:c>
     </x:row>
-    <x:row r="10" spans="1:46">
+    <x:row r="10" spans="1:47">
       <x:c r="A10" s="3" t="s">
-        <x:v>53</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="B10" s="4" t="n">
         <x:v>1</x:v>
@@ -2423,10 +2447,13 @@
       <x:c r="AT10" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU10" s="4" t="n">
+        <x:v>3</x:v>
+      </x:c>
     </x:row>
-    <x:row r="11" spans="1:46">
+    <x:row r="11" spans="1:47">
       <x:c r="A11" s="3" t="s">
-        <x:v>54</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="B11" s="4" t="n">
         <x:v>0</x:v>
@@ -2563,10 +2590,13 @@
       <x:c r="AT11" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU11" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="12" spans="1:46">
+    <x:row r="12" spans="1:47">
       <x:c r="A12" s="3" t="s">
-        <x:v>55</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="B12" s="4" t="n">
         <x:v>0</x:v>
@@ -2703,10 +2733,13 @@
       <x:c r="AT12" s="4" t="n">
         <x:v>7</x:v>
       </x:c>
+      <x:c r="AU12" s="4" t="n">
+        <x:v>14</x:v>
+      </x:c>
     </x:row>
-    <x:row r="13" spans="1:46">
+    <x:row r="13" spans="1:47">
       <x:c r="A13" s="3" t="s">
-        <x:v>56</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="B13" s="4" t="n">
         <x:v>87</x:v>
@@ -2843,10 +2876,13 @@
       <x:c r="AT13" s="4" t="n">
         <x:v>31</x:v>
       </x:c>
+      <x:c r="AU13" s="4" t="n">
+        <x:v>31</x:v>
+      </x:c>
     </x:row>
-    <x:row r="14" spans="1:46">
+    <x:row r="14" spans="1:47">
       <x:c r="A14" s="3" t="s">
-        <x:v>57</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="B14" s="4" t="n">
         <x:v>123</x:v>
@@ -2983,10 +3019,13 @@
       <x:c r="AT14" s="4" t="n">
         <x:v>18</x:v>
       </x:c>
+      <x:c r="AU14" s="4" t="n">
+        <x:v>50</x:v>
+      </x:c>
     </x:row>
-    <x:row r="15" spans="1:46">
+    <x:row r="15" spans="1:47">
       <x:c r="A15" s="3" t="s">
-        <x:v>58</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="B15" s="4" t="n">
         <x:v>79</x:v>
@@ -3123,10 +3162,13 @@
       <x:c r="AT15" s="4" t="n">
         <x:v>5</x:v>
       </x:c>
+      <x:c r="AU15" s="4" t="n">
+        <x:v>35</x:v>
+      </x:c>
     </x:row>
-    <x:row r="16" spans="1:46">
+    <x:row r="16" spans="1:47">
       <x:c r="A16" s="3" t="s">
-        <x:v>59</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="B16" s="4" t="n">
         <x:v>14</x:v>
@@ -3263,10 +3305,13 @@
       <x:c r="AT16" s="4" t="n">
         <x:v>7</x:v>
       </x:c>
+      <x:c r="AU16" s="4" t="n">
+        <x:v>21</x:v>
+      </x:c>
     </x:row>
-    <x:row r="17" spans="1:46">
+    <x:row r="17" spans="1:47">
       <x:c r="A17" s="3" t="s">
-        <x:v>60</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="B17" s="4" t="n">
         <x:v>57</x:v>
@@ -3403,10 +3448,13 @@
       <x:c r="AT17" s="4" t="n">
         <x:v>70</x:v>
       </x:c>
+      <x:c r="AU17" s="4" t="n">
+        <x:v>70</x:v>
+      </x:c>
     </x:row>
-    <x:row r="18" spans="1:46">
+    <x:row r="18" spans="1:47">
       <x:c r="A18" s="3" t="s">
-        <x:v>61</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="B18" s="4" t="n">
         <x:v>178</x:v>
@@ -3543,10 +3591,13 @@
       <x:c r="AT18" s="4" t="n">
         <x:v>35</x:v>
       </x:c>
+      <x:c r="AU18" s="4" t="n">
+        <x:v>67</x:v>
+      </x:c>
     </x:row>
-    <x:row r="19" spans="1:46">
+    <x:row r="19" spans="1:47">
       <x:c r="A19" s="3" t="s">
-        <x:v>62</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="B19" s="4" t="n">
         <x:v>72</x:v>
@@ -3683,10 +3734,13 @@
       <x:c r="AT19" s="4" t="n">
         <x:v>13</x:v>
       </x:c>
+      <x:c r="AU19" s="4" t="n">
+        <x:v>7</x:v>
+      </x:c>
     </x:row>
-    <x:row r="20" spans="1:46">
+    <x:row r="20" spans="1:47">
       <x:c r="A20" s="3" t="s">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="B20" s="4" t="n">
         <x:v>0</x:v>
@@ -3823,10 +3877,13 @@
       <x:c r="AT20" s="4" t="n">
         <x:v>3</x:v>
       </x:c>
+      <x:c r="AU20" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="21" spans="1:46">
+    <x:row r="21" spans="1:47">
       <x:c r="A21" s="3" t="s">
-        <x:v>64</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="B21" s="4" t="n">
         <x:v>0</x:v>
@@ -3963,10 +4020,13 @@
       <x:c r="AT21" s="4" t="n">
         <x:v>33</x:v>
       </x:c>
+      <x:c r="AU21" s="4" t="n">
+        <x:v>38</x:v>
+      </x:c>
     </x:row>
-    <x:row r="22" spans="1:46">
+    <x:row r="22" spans="1:47">
       <x:c r="A22" s="3" t="s">
-        <x:v>65</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="B22" s="4" t="n">
         <x:v>0</x:v>
@@ -4103,10 +4163,13 @@
       <x:c r="AT22" s="4" t="n">
         <x:v>5</x:v>
       </x:c>
+      <x:c r="AU22" s="4" t="n">
+        <x:v>20</x:v>
+      </x:c>
     </x:row>
-    <x:row r="23" spans="1:46">
+    <x:row r="23" spans="1:47">
       <x:c r="A23" s="3" t="s">
-        <x:v>66</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="B23" s="4" t="n">
         <x:v>0</x:v>
@@ -4243,10 +4306,13 @@
       <x:c r="AT23" s="4" t="n">
         <x:v>29</x:v>
       </x:c>
+      <x:c r="AU23" s="4" t="n">
+        <x:v>58</x:v>
+      </x:c>
     </x:row>
-    <x:row r="24" spans="1:46">
+    <x:row r="24" spans="1:47">
       <x:c r="A24" s="3" t="s">
-        <x:v>67</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="B24" s="4" t="n">
         <x:v>0</x:v>
@@ -4383,10 +4449,13 @@
       <x:c r="AT24" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU24" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="25" spans="1:46">
+    <x:row r="25" spans="1:47">
       <x:c r="A25" s="3" t="s">
-        <x:v>68</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="B25" s="4" t="n">
         <x:v>0</x:v>
@@ -4523,10 +4592,13 @@
       <x:c r="AT25" s="4" t="n">
         <x:v>30</x:v>
       </x:c>
+      <x:c r="AU25" s="4" t="n">
+        <x:v>89</x:v>
+      </x:c>
     </x:row>
-    <x:row r="26" spans="1:46">
+    <x:row r="26" spans="1:47">
       <x:c r="A26" s="3" t="s">
-        <x:v>69</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="B26" s="4" t="n">
         <x:v>1</x:v>
@@ -4663,10 +4735,13 @@
       <x:c r="AT26" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU26" s="4" t="n">
+        <x:v>1</x:v>
+      </x:c>
     </x:row>
-    <x:row r="27" spans="1:46">
+    <x:row r="27" spans="1:47">
       <x:c r="A27" s="3" t="s">
-        <x:v>70</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="B27" s="4" t="n">
         <x:v>3</x:v>
@@ -4803,10 +4878,13 @@
       <x:c r="AT27" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU27" s="4" t="n">
+        <x:v>2</x:v>
+      </x:c>
     </x:row>
-    <x:row r="28" spans="1:46">
+    <x:row r="28" spans="1:47">
       <x:c r="A28" s="3" t="s">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="B28" s="4" t="n">
         <x:v>0</x:v>
@@ -4943,10 +5021,13 @@
       <x:c r="AT28" s="4" t="n">
         <x:v>5</x:v>
       </x:c>
+      <x:c r="AU28" s="4" t="n">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
-    <x:row r="29" spans="1:46">
+    <x:row r="29" spans="1:47">
       <x:c r="A29" s="3" t="s">
-        <x:v>72</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="B29" s="4" t="n">
         <x:v>0</x:v>
@@ -5083,10 +5164,13 @@
       <x:c r="AT29" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU29" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="30" spans="1:46">
+    <x:row r="30" spans="1:47">
       <x:c r="A30" s="3" t="s">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="B30" s="4" t="n">
         <x:v>0</x:v>
@@ -5223,10 +5307,13 @@
       <x:c r="AT30" s="4" t="n">
         <x:v>5</x:v>
       </x:c>
+      <x:c r="AU30" s="4" t="n">
+        <x:v>10</x:v>
+      </x:c>
     </x:row>
-    <x:row r="31" spans="1:46">
+    <x:row r="31" spans="1:47">
       <x:c r="A31" s="3" t="s">
-        <x:v>74</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="B31" s="4" t="n">
         <x:v>131</x:v>
@@ -5363,10 +5450,13 @@
       <x:c r="AT31" s="4" t="n">
         <x:v>25</x:v>
       </x:c>
+      <x:c r="AU31" s="4" t="n">
+        <x:v>39</x:v>
+      </x:c>
     </x:row>
-    <x:row r="32" spans="1:46">
+    <x:row r="32" spans="1:47">
       <x:c r="A32" s="3" t="s">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="B32" s="4" t="n">
         <x:v>0</x:v>
@@ -5503,10 +5593,13 @@
       <x:c r="AT32" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU32" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="33" spans="1:46">
+    <x:row r="33" spans="1:47">
       <x:c r="A33" s="3" t="s">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="B33" s="4" t="n">
         <x:v>0</x:v>
@@ -5643,10 +5736,13 @@
       <x:c r="AT33" s="4" t="n">
         <x:v>30</x:v>
       </x:c>
+      <x:c r="AU33" s="4" t="n">
+        <x:v>40</x:v>
+      </x:c>
     </x:row>
-    <x:row r="34" spans="1:46">
+    <x:row r="34" spans="1:47">
       <x:c r="A34" s="3" t="s">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="B34" s="4" t="n">
         <x:v>338</x:v>
@@ -5783,10 +5879,13 @@
       <x:c r="AT34" s="4" t="n">
         <x:v>119</x:v>
       </x:c>
+      <x:c r="AU34" s="4" t="n">
+        <x:v>94</x:v>
+      </x:c>
     </x:row>
-    <x:row r="35" spans="1:46">
+    <x:row r="35" spans="1:47">
       <x:c r="A35" s="3" t="s">
-        <x:v>78</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="B35" s="4" t="n">
         <x:v>162</x:v>
@@ -5923,10 +6022,13 @@
       <x:c r="AT35" s="4" t="n">
         <x:v>143</x:v>
       </x:c>
+      <x:c r="AU35" s="4" t="n">
+        <x:v>255</x:v>
+      </x:c>
     </x:row>
-    <x:row r="36" spans="1:46">
+    <x:row r="36" spans="1:47">
       <x:c r="A36" s="3" t="s">
-        <x:v>79</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="B36" s="4" t="n">
         <x:v>40</x:v>
@@ -6063,10 +6165,13 @@
       <x:c r="AT36" s="4" t="n">
         <x:v>5</x:v>
       </x:c>
+      <x:c r="AU36" s="4" t="n">
+        <x:v>14</x:v>
+      </x:c>
     </x:row>
-    <x:row r="37" spans="1:46">
+    <x:row r="37" spans="1:47">
       <x:c r="A37" s="3" t="s">
-        <x:v>80</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="B37" s="4" t="n">
         <x:v>6</x:v>
@@ -6203,10 +6308,13 @@
       <x:c r="AT37" s="4" t="n">
         <x:v>131</x:v>
       </x:c>
+      <x:c r="AU37" s="4" t="n">
+        <x:v>244</x:v>
+      </x:c>
     </x:row>
-    <x:row r="38" spans="1:46">
+    <x:row r="38" spans="1:47">
       <x:c r="A38" s="3" t="s">
-        <x:v>81</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="B38" s="4" t="n">
         <x:v>0</x:v>
@@ -6343,10 +6451,13 @@
       <x:c r="AT38" s="4" t="n">
         <x:v>54</x:v>
       </x:c>
+      <x:c r="AU38" s="4" t="n">
+        <x:v>125</x:v>
+      </x:c>
     </x:row>
-    <x:row r="39" spans="1:46">
+    <x:row r="39" spans="1:47">
       <x:c r="A39" s="3" t="s">
-        <x:v>82</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="B39" s="4" t="n">
         <x:v>0</x:v>
@@ -6483,10 +6594,13 @@
       <x:c r="AT39" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU39" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="40" spans="1:46">
+    <x:row r="40" spans="1:47">
       <x:c r="A40" s="3" t="s">
-        <x:v>83</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="B40" s="4" t="n">
         <x:v>79</x:v>
@@ -6623,10 +6737,13 @@
       <x:c r="AT40" s="4" t="n">
         <x:v>7</x:v>
       </x:c>
+      <x:c r="AU40" s="4" t="n">
+        <x:v>22</x:v>
+      </x:c>
     </x:row>
-    <x:row r="41" spans="1:46">
+    <x:row r="41" spans="1:47">
       <x:c r="A41" s="3" t="s">
-        <x:v>84</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="B41" s="4" t="n">
         <x:v>0</x:v>
@@ -6763,10 +6880,13 @@
       <x:c r="AT41" s="4" t="n">
         <x:v>14</x:v>
       </x:c>
+      <x:c r="AU41" s="4" t="n">
+        <x:v>57</x:v>
+      </x:c>
     </x:row>
-    <x:row r="42" spans="1:46">
+    <x:row r="42" spans="1:47">
       <x:c r="A42" s="3" t="s">
-        <x:v>85</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="B42" s="4" t="n">
         <x:v>0</x:v>
@@ -6903,10 +7023,13 @@
       <x:c r="AT42" s="4" t="n">
         <x:v>3</x:v>
       </x:c>
+      <x:c r="AU42" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="43" spans="1:46">
+    <x:row r="43" spans="1:47">
       <x:c r="A43" s="3" t="s">
-        <x:v>86</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="B43" s="4" t="n">
         <x:v>0</x:v>
@@ -7043,10 +7166,13 @@
       <x:c r="AT43" s="4" t="n">
         <x:v>6</x:v>
       </x:c>
+      <x:c r="AU43" s="4" t="n">
+        <x:v>29</x:v>
+      </x:c>
     </x:row>
-    <x:row r="44" spans="1:46">
+    <x:row r="44" spans="1:47">
       <x:c r="A44" s="3" t="s">
-        <x:v>87</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="B44" s="4" t="n">
         <x:v>0</x:v>
@@ -7183,10 +7309,13 @@
       <x:c r="AT44" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU44" s="4" t="n">
+        <x:v>2</x:v>
+      </x:c>
     </x:row>
-    <x:row r="45" spans="1:46">
+    <x:row r="45" spans="1:47">
       <x:c r="A45" s="3" t="s">
-        <x:v>88</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="B45" s="4" t="n">
         <x:v>6</x:v>
@@ -7323,10 +7452,13 @@
       <x:c r="AT45" s="4" t="n">
         <x:v>1</x:v>
       </x:c>
+      <x:c r="AU45" s="4" t="n">
+        <x:v>2</x:v>
+      </x:c>
     </x:row>
-    <x:row r="46" spans="1:46">
+    <x:row r="46" spans="1:47">
       <x:c r="A46" s="3" t="s">
-        <x:v>89</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="B46" s="4" t="n">
         <x:v>125</x:v>
@@ -7463,10 +7595,13 @@
       <x:c r="AT46" s="4" t="n">
         <x:v>39</x:v>
       </x:c>
+      <x:c r="AU46" s="4" t="n">
+        <x:v>61</x:v>
+      </x:c>
     </x:row>
-    <x:row r="47" spans="1:46">
+    <x:row r="47" spans="1:47">
       <x:c r="A47" s="3" t="s">
-        <x:v>90</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="B47" s="4" t="n">
         <x:v>464</x:v>
@@ -7603,10 +7738,13 @@
       <x:c r="AT47" s="4" t="n">
         <x:v>202</x:v>
       </x:c>
+      <x:c r="AU47" s="4" t="n">
+        <x:v>362</x:v>
+      </x:c>
     </x:row>
-    <x:row r="48" spans="1:46">
+    <x:row r="48" spans="1:47">
       <x:c r="A48" s="3" t="s">
-        <x:v>91</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="B48" s="4" t="n">
         <x:v>194</x:v>
@@ -7743,10 +7881,13 @@
       <x:c r="AT48" s="4" t="n">
         <x:v>129</x:v>
       </x:c>
+      <x:c r="AU48" s="4" t="n">
+        <x:v>152</x:v>
+      </x:c>
     </x:row>
-    <x:row r="49" spans="1:46">
+    <x:row r="49" spans="1:47">
       <x:c r="A49" s="3" t="s">
-        <x:v>92</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="B49" s="4" t="n">
         <x:v>0</x:v>
@@ -7883,10 +8024,13 @@
       <x:c r="AT49" s="4" t="n">
         <x:v>10</x:v>
       </x:c>
+      <x:c r="AU49" s="4" t="n">
+        <x:v>16</x:v>
+      </x:c>
     </x:row>
-    <x:row r="50" spans="1:46">
+    <x:row r="50" spans="1:47">
       <x:c r="A50" s="3" t="s">
-        <x:v>93</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="B50" s="4" t="n">
         <x:v>28</x:v>
@@ -8023,10 +8167,13 @@
       <x:c r="AT50" s="4" t="n">
         <x:v>1</x:v>
       </x:c>
+      <x:c r="AU50" s="4" t="n">
+        <x:v>2</x:v>
+      </x:c>
     </x:row>
-    <x:row r="51" spans="1:46">
+    <x:row r="51" spans="1:47">
       <x:c r="A51" s="3" t="s">
-        <x:v>94</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="B51" s="4" t="n">
         <x:v>98</x:v>
@@ -8163,10 +8310,13 @@
       <x:c r="AT51" s="4" t="n">
         <x:v>83</x:v>
       </x:c>
+      <x:c r="AU51" s="4" t="n">
+        <x:v>176</x:v>
+      </x:c>
     </x:row>
-    <x:row r="52" spans="1:46">
+    <x:row r="52" spans="1:47">
       <x:c r="A52" s="3" t="s">
-        <x:v>95</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="B52" s="4" t="n">
         <x:v>1129</x:v>
@@ -8303,10 +8453,13 @@
       <x:c r="AT52" s="4" t="n">
         <x:v>159</x:v>
       </x:c>
+      <x:c r="AU52" s="4" t="n">
+        <x:v>315</x:v>
+      </x:c>
     </x:row>
-    <x:row r="53" spans="1:46">
+    <x:row r="53" spans="1:47">
       <x:c r="A53" s="3" t="s">
-        <x:v>96</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="B53" s="4" t="n">
         <x:v>0</x:v>
@@ -8443,10 +8596,13 @@
       <x:c r="AT53" s="4" t="n">
         <x:v>144</x:v>
       </x:c>
+      <x:c r="AU53" s="4" t="n">
+        <x:v>289</x:v>
+      </x:c>
     </x:row>
-    <x:row r="54" spans="1:46">
+    <x:row r="54" spans="1:47">
       <x:c r="A54" s="3" t="s">
-        <x:v>97</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="B54" s="4" t="n">
         <x:v>42</x:v>
@@ -8583,10 +8739,13 @@
       <x:c r="AT54" s="4" t="n">
         <x:v>29</x:v>
       </x:c>
+      <x:c r="AU54" s="4" t="n">
+        <x:v>67</x:v>
+      </x:c>
     </x:row>
-    <x:row r="55" spans="1:46">
+    <x:row r="55" spans="1:47">
       <x:c r="A55" s="3" t="s">
-        <x:v>98</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="B55" s="4" t="n">
         <x:v>0</x:v>
@@ -8723,10 +8882,13 @@
       <x:c r="AT55" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU55" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="56" spans="1:46">
+    <x:row r="56" spans="1:47">
       <x:c r="A56" s="3" t="s">
-        <x:v>99</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="B56" s="4" t="n">
         <x:v>90</x:v>
@@ -8863,10 +9025,13 @@
       <x:c r="AT56" s="4" t="n">
         <x:v>5</x:v>
       </x:c>
+      <x:c r="AU56" s="4" t="n">
+        <x:v>2</x:v>
+      </x:c>
     </x:row>
-    <x:row r="57" spans="1:46">
+    <x:row r="57" spans="1:47">
       <x:c r="A57" s="3" t="s">
-        <x:v>100</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="B57" s="4" t="n">
         <x:v>0</x:v>
@@ -9003,10 +9168,13 @@
       <x:c r="AT57" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU57" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="58" spans="1:46">
+    <x:row r="58" spans="1:47">
       <x:c r="A58" s="3" t="s">
-        <x:v>101</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="B58" s="4" t="n">
         <x:v>54</x:v>
@@ -9143,10 +9311,13 @@
       <x:c r="AT58" s="4" t="n">
         <x:v>6</x:v>
       </x:c>
+      <x:c r="AU58" s="4" t="n">
+        <x:v>3</x:v>
+      </x:c>
     </x:row>
-    <x:row r="59" spans="1:46">
+    <x:row r="59" spans="1:47">
       <x:c r="A59" s="3" t="s">
-        <x:v>102</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="B59" s="4" t="n">
         <x:v>0</x:v>
@@ -9283,10 +9454,13 @@
       <x:c r="AT59" s="4" t="n">
         <x:v>2</x:v>
       </x:c>
+      <x:c r="AU59" s="4" t="n">
+        <x:v>1</x:v>
+      </x:c>
     </x:row>
-    <x:row r="60" spans="1:46">
+    <x:row r="60" spans="1:47">
       <x:c r="A60" s="3" t="s">
-        <x:v>103</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="B60" s="4" t="n">
         <x:v>0</x:v>
@@ -9423,10 +9597,13 @@
       <x:c r="AT60" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU60" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="61" spans="1:46">
+    <x:row r="61" spans="1:47">
       <x:c r="A61" s="3" t="s">
-        <x:v>104</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="B61" s="4" t="n">
         <x:v>0</x:v>
@@ -9563,10 +9740,13 @@
       <x:c r="AT61" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU61" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="62" spans="1:46">
+    <x:row r="62" spans="1:47">
       <x:c r="A62" s="3" t="s">
-        <x:v>105</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="B62" s="4" t="n">
         <x:v>0</x:v>
@@ -9703,10 +9883,13 @@
       <x:c r="AT62" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU62" s="4" t="n">
+        <x:v>1</x:v>
+      </x:c>
     </x:row>
-    <x:row r="63" spans="1:46">
+    <x:row r="63" spans="1:47">
       <x:c r="A63" s="3" t="s">
-        <x:v>106</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="B63" s="4" t="n">
         <x:v>1</x:v>
@@ -9843,10 +10026,13 @@
       <x:c r="AT63" s="4" t="n">
         <x:v>3</x:v>
       </x:c>
+      <x:c r="AU63" s="4" t="n">
+        <x:v>6</x:v>
+      </x:c>
     </x:row>
-    <x:row r="64" spans="1:46">
+    <x:row r="64" spans="1:47">
       <x:c r="A64" s="3" t="s">
-        <x:v>107</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="B64" s="4" t="n">
         <x:v>0</x:v>
@@ -9983,10 +10169,13 @@
       <x:c r="AT64" s="4" t="n">
         <x:v>15</x:v>
       </x:c>
+      <x:c r="AU64" s="4" t="n">
+        <x:v>50</x:v>
+      </x:c>
     </x:row>
-    <x:row r="65" spans="1:46">
+    <x:row r="65" spans="1:47">
       <x:c r="A65" s="3" t="s">
-        <x:v>108</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="B65" s="4" t="n">
         <x:v>0</x:v>
@@ -10123,10 +10312,13 @@
       <x:c r="AT65" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU65" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="66" spans="1:46">
+    <x:row r="66" spans="1:47">
       <x:c r="A66" s="3" t="s">
-        <x:v>109</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="B66" s="4" t="n">
         <x:v>0</x:v>
@@ -10263,10 +10455,13 @@
       <x:c r="AT66" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU66" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="67" spans="1:46">
+    <x:row r="67" spans="1:47">
       <x:c r="A67" s="3" t="s">
-        <x:v>110</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="B67" s="4" t="n">
         <x:v>2</x:v>
@@ -10403,10 +10598,13 @@
       <x:c r="AT67" s="4" t="n">
         <x:v>17</x:v>
       </x:c>
+      <x:c r="AU67" s="4" t="n">
+        <x:v>25</x:v>
+      </x:c>
     </x:row>
-    <x:row r="68" spans="1:46">
+    <x:row r="68" spans="1:47">
       <x:c r="A68" s="3" t="s">
-        <x:v>111</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="B68" s="4" t="n">
         <x:v>0</x:v>
@@ -10543,10 +10741,13 @@
       <x:c r="AT68" s="4" t="n">
         <x:v>4</x:v>
       </x:c>
+      <x:c r="AU68" s="4" t="n">
+        <x:v>2</x:v>
+      </x:c>
     </x:row>
-    <x:row r="69" spans="1:46">
+    <x:row r="69" spans="1:47">
       <x:c r="A69" s="3" t="s">
-        <x:v>112</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="B69" s="4" t="n">
         <x:v>0</x:v>
@@ -10683,10 +10884,13 @@
       <x:c r="AT69" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU69" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="70" spans="1:46">
+    <x:row r="70" spans="1:47">
       <x:c r="A70" s="3" t="s">
-        <x:v>113</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="B70" s="4" t="n">
         <x:v>118</x:v>
@@ -10823,10 +11027,13 @@
       <x:c r="AT70" s="4" t="n">
         <x:v>4</x:v>
       </x:c>
+      <x:c r="AU70" s="4" t="n">
+        <x:v>22</x:v>
+      </x:c>
     </x:row>
-    <x:row r="71" spans="1:46">
+    <x:row r="71" spans="1:47">
       <x:c r="A71" s="3" t="s">
-        <x:v>114</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="B71" s="4" t="n">
         <x:v>0</x:v>
@@ -10963,10 +11170,13 @@
       <x:c r="AT71" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU71" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="72" spans="1:46">
+    <x:row r="72" spans="1:47">
       <x:c r="A72" s="3" t="s">
-        <x:v>115</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="B72" s="4" t="n">
         <x:v>0</x:v>
@@ -11103,10 +11313,13 @@
       <x:c r="AT72" s="4" t="n">
         <x:v>2</x:v>
       </x:c>
+      <x:c r="AU72" s="4" t="n">
+        <x:v>10</x:v>
+      </x:c>
     </x:row>
-    <x:row r="73" spans="1:46">
+    <x:row r="73" spans="1:47">
       <x:c r="A73" s="3" t="s">
-        <x:v>116</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="B73" s="4" t="n">
         <x:v>1</x:v>
@@ -11243,10 +11456,13 @@
       <x:c r="AT73" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU73" s="4" t="n">
+        <x:v>1</x:v>
+      </x:c>
     </x:row>
-    <x:row r="74" spans="1:46">
+    <x:row r="74" spans="1:47">
       <x:c r="A74" s="3" t="s">
-        <x:v>117</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="B74" s="4" t="n">
         <x:v>13</x:v>
@@ -11383,10 +11599,13 @@
       <x:c r="AT74" s="4" t="n">
         <x:v>4</x:v>
       </x:c>
+      <x:c r="AU74" s="4" t="n">
+        <x:v>22</x:v>
+      </x:c>
     </x:row>
-    <x:row r="75" spans="1:46">
+    <x:row r="75" spans="1:47">
       <x:c r="A75" s="3" t="s">
-        <x:v>118</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="B75" s="4" t="n">
         <x:v>0</x:v>
@@ -11523,10 +11742,13 @@
       <x:c r="AT75" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU75" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="76" spans="1:46">
+    <x:row r="76" spans="1:47">
       <x:c r="A76" s="3" t="s">
-        <x:v>119</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="B76" s="4" t="n">
         <x:v>9</x:v>
@@ -11663,10 +11885,13 @@
       <x:c r="AT76" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU76" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="77" spans="1:46">
+    <x:row r="77" spans="1:47">
       <x:c r="A77" s="3" t="s">
-        <x:v>120</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="B77" s="4" t="n">
         <x:v>34</x:v>
@@ -11803,10 +12028,13 @@
       <x:c r="AT77" s="4" t="n">
         <x:v>11</x:v>
       </x:c>
+      <x:c r="AU77" s="4" t="n">
+        <x:v>24</x:v>
+      </x:c>
     </x:row>
-    <x:row r="78" spans="1:46">
+    <x:row r="78" spans="1:47">
       <x:c r="A78" s="3" t="s">
-        <x:v>121</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="B78" s="4" t="n">
         <x:v>0</x:v>
@@ -11943,10 +12171,13 @@
       <x:c r="AT78" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU78" s="4" t="n">
+        <x:v>3</x:v>
+      </x:c>
     </x:row>
-    <x:row r="79" spans="1:46">
+    <x:row r="79" spans="1:47">
       <x:c r="A79" s="3" t="s">
-        <x:v>122</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="B79" s="4" t="n">
         <x:v>0</x:v>
@@ -12083,10 +12314,13 @@
       <x:c r="AT79" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU79" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="80" spans="1:46">
+    <x:row r="80" spans="1:47">
       <x:c r="A80" s="3" t="s">
-        <x:v>123</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="B80" s="4" t="n">
         <x:v>0</x:v>
@@ -12223,10 +12457,13 @@
       <x:c r="AT80" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU80" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="81" spans="1:46">
+    <x:row r="81" spans="1:47">
       <x:c r="A81" s="3" t="s">
-        <x:v>124</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="B81" s="4" t="n">
         <x:v>7</x:v>
@@ -12363,10 +12600,13 @@
       <x:c r="AT81" s="4" t="n">
         <x:v>12</x:v>
       </x:c>
+      <x:c r="AU81" s="4" t="n">
+        <x:v>6</x:v>
+      </x:c>
     </x:row>
-    <x:row r="82" spans="1:46">
+    <x:row r="82" spans="1:47">
       <x:c r="A82" s="3" t="s">
-        <x:v>125</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="B82" s="4" t="n">
         <x:v>0</x:v>
@@ -12503,10 +12743,13 @@
       <x:c r="AT82" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU82" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="83" spans="1:46">
+    <x:row r="83" spans="1:47">
       <x:c r="A83" s="3" t="s">
-        <x:v>126</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="B83" s="4" t="n">
         <x:v>2</x:v>
@@ -12643,10 +12886,13 @@
       <x:c r="AT83" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU83" s="4" t="n">
+        <x:v>3</x:v>
+      </x:c>
     </x:row>
-    <x:row r="84" spans="1:46">
+    <x:row r="84" spans="1:47">
       <x:c r="A84" s="3" t="s">
-        <x:v>127</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="B84" s="4" t="n">
         <x:v>9</x:v>
@@ -12783,10 +13029,13 @@
       <x:c r="AT84" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU84" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="85" spans="1:46">
+    <x:row r="85" spans="1:47">
       <x:c r="A85" s="3" t="s">
-        <x:v>128</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="B85" s="4" t="n">
         <x:v>0</x:v>
@@ -12923,10 +13172,13 @@
       <x:c r="AT85" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU85" s="4" t="n">
+        <x:v>1</x:v>
+      </x:c>
     </x:row>
-    <x:row r="86" spans="1:46">
+    <x:row r="86" spans="1:47">
       <x:c r="A86" s="3" t="s">
-        <x:v>129</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="B86" s="4" t="n">
         <x:v>2</x:v>
@@ -13063,10 +13315,13 @@
       <x:c r="AT86" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU86" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="87" spans="1:46">
+    <x:row r="87" spans="1:47">
       <x:c r="A87" s="3" t="s">
-        <x:v>130</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="B87" s="4" t="n">
         <x:v>0</x:v>
@@ -13203,10 +13458,13 @@
       <x:c r="AT87" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU87" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="88" spans="1:46">
+    <x:row r="88" spans="1:47">
       <x:c r="A88" s="3" t="s">
-        <x:v>131</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="B88" s="4" t="n">
         <x:v>40</x:v>
@@ -13343,10 +13601,13 @@
       <x:c r="AT88" s="4" t="n">
         <x:v>11</x:v>
       </x:c>
+      <x:c r="AU88" s="4" t="n">
+        <x:v>26</x:v>
+      </x:c>
     </x:row>
-    <x:row r="89" spans="1:46">
+    <x:row r="89" spans="1:47">
       <x:c r="A89" s="3" t="s">
-        <x:v>132</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="B89" s="4" t="n">
         <x:v>2</x:v>
@@ -13483,10 +13744,13 @@
       <x:c r="AT89" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU89" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="90" spans="1:46">
+    <x:row r="90" spans="1:47">
       <x:c r="A90" s="3" t="s">
-        <x:v>133</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="B90" s="4" t="n">
         <x:v>13</x:v>
@@ -13623,10 +13887,13 @@
       <x:c r="AT90" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU90" s="4" t="n">
+        <x:v>1</x:v>
+      </x:c>
     </x:row>
-    <x:row r="91" spans="1:46">
+    <x:row r="91" spans="1:47">
       <x:c r="A91" s="3" t="s">
-        <x:v>134</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="B91" s="4" t="n">
         <x:v>0</x:v>
@@ -13763,10 +14030,13 @@
       <x:c r="AT91" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU91" s="4" t="n">
+        <x:v>1</x:v>
+      </x:c>
     </x:row>
-    <x:row r="92" spans="1:46">
+    <x:row r="92" spans="1:47">
       <x:c r="A92" s="3" t="s">
-        <x:v>135</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="B92" s="4" t="n">
         <x:v>0</x:v>
@@ -13903,10 +14173,13 @@
       <x:c r="AT92" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU92" s="4" t="n">
+        <x:v>2</x:v>
+      </x:c>
     </x:row>
-    <x:row r="93" spans="1:46">
+    <x:row r="93" spans="1:47">
       <x:c r="A93" s="3" t="s">
-        <x:v>136</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="B93" s="4" t="n">
         <x:v>0</x:v>
@@ -14043,10 +14316,13 @@
       <x:c r="AT93" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU93" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="94" spans="1:46">
+    <x:row r="94" spans="1:47">
       <x:c r="A94" s="3" t="s">
-        <x:v>137</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="B94" s="4" t="n">
         <x:v>10</x:v>
@@ -14183,10 +14459,13 @@
       <x:c r="AT94" s="4" t="n">
         <x:v>24</x:v>
       </x:c>
+      <x:c r="AU94" s="4" t="n">
+        <x:v>47</x:v>
+      </x:c>
     </x:row>
-    <x:row r="95" spans="1:46">
+    <x:row r="95" spans="1:47">
       <x:c r="A95" s="3" t="s">
-        <x:v>138</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="B95" s="4" t="n">
         <x:v>0</x:v>
@@ -14323,10 +14602,13 @@
       <x:c r="AT95" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU95" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="96" spans="1:46">
+    <x:row r="96" spans="1:47">
       <x:c r="A96" s="3" t="s">
-        <x:v>139</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="B96" s="4" t="n">
         <x:v>0</x:v>
@@ -14463,10 +14745,13 @@
       <x:c r="AT96" s="4" t="n">
         <x:v>1</x:v>
       </x:c>
+      <x:c r="AU96" s="4" t="n">
+        <x:v>2</x:v>
+      </x:c>
     </x:row>
-    <x:row r="97" spans="1:46">
+    <x:row r="97" spans="1:47">
       <x:c r="A97" s="3" t="s">
-        <x:v>140</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="B97" s="4" t="n">
         <x:v>0</x:v>
@@ -14603,10 +14888,13 @@
       <x:c r="AT97" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU97" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="98" spans="1:46">
+    <x:row r="98" spans="1:47">
       <x:c r="A98" s="3" t="s">
-        <x:v>141</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="B98" s="4" t="n">
         <x:v>1</x:v>
@@ -14743,10 +15031,13 @@
       <x:c r="AT98" s="4" t="n">
         <x:v>4</x:v>
       </x:c>
+      <x:c r="AU98" s="4" t="n">
+        <x:v>2</x:v>
+      </x:c>
     </x:row>
-    <x:row r="99" spans="1:46">
+    <x:row r="99" spans="1:47">
       <x:c r="A99" s="3" t="s">
-        <x:v>142</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="B99" s="4" t="n">
         <x:v>0</x:v>
@@ -14883,10 +15174,13 @@
       <x:c r="AT99" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU99" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="100" spans="1:46">
+    <x:row r="100" spans="1:47">
       <x:c r="A100" s="3" t="s">
-        <x:v>143</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="B100" s="4" t="n">
         <x:v>0</x:v>
@@ -15023,10 +15317,13 @@
       <x:c r="AT100" s="4" t="n">
         <x:v>3</x:v>
       </x:c>
+      <x:c r="AU100" s="4" t="n">
+        <x:v>4</x:v>
+      </x:c>
     </x:row>
-    <x:row r="101" spans="1:46">
+    <x:row r="101" spans="1:47">
       <x:c r="A101" s="3" t="s">
-        <x:v>144</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="B101" s="4" t="n">
         <x:v>0</x:v>
@@ -15163,10 +15460,13 @@
       <x:c r="AT101" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU101" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="102" spans="1:46">
+    <x:row r="102" spans="1:47">
       <x:c r="A102" s="3" t="s">
-        <x:v>145</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="B102" s="4" t="n">
         <x:v>14</x:v>
@@ -15303,10 +15603,13 @@
       <x:c r="AT102" s="4" t="n">
         <x:v>73</x:v>
       </x:c>
+      <x:c r="AU102" s="4" t="n">
+        <x:v>83</x:v>
+      </x:c>
     </x:row>
-    <x:row r="103" spans="1:46">
+    <x:row r="103" spans="1:47">
       <x:c r="A103" s="3" t="s">
-        <x:v>146</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="B103" s="4" t="n">
         <x:v>0</x:v>
@@ -15443,10 +15746,13 @@
       <x:c r="AT103" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU103" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="104" spans="1:46">
+    <x:row r="104" spans="1:47">
       <x:c r="A104" s="3" t="s">
-        <x:v>147</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="B104" s="4" t="n">
         <x:v>11</x:v>
@@ -15583,10 +15889,13 @@
       <x:c r="AT104" s="4" t="n">
         <x:v>12</x:v>
       </x:c>
+      <x:c r="AU104" s="4" t="n">
+        <x:v>6</x:v>
+      </x:c>
     </x:row>
-    <x:row r="105" spans="1:46">
+    <x:row r="105" spans="1:47">
       <x:c r="A105" s="3" t="s">
-        <x:v>148</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="B105" s="4" t="n">
         <x:v>9</x:v>
@@ -15723,10 +16032,13 @@
       <x:c r="AT105" s="4" t="n">
         <x:v>10</x:v>
       </x:c>
+      <x:c r="AU105" s="4" t="n">
+        <x:v>20</x:v>
+      </x:c>
     </x:row>
-    <x:row r="106" spans="1:46">
+    <x:row r="106" spans="1:47">
       <x:c r="A106" s="3" t="s">
-        <x:v>149</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="B106" s="4" t="n">
         <x:v>0</x:v>
@@ -15863,10 +16175,13 @@
       <x:c r="AT106" s="4" t="n">
         <x:v>3</x:v>
       </x:c>
+      <x:c r="AU106" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="107" spans="1:46">
+    <x:row r="107" spans="1:47">
       <x:c r="A107" s="3" t="s">
-        <x:v>150</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="B107" s="4" t="n">
         <x:v>0</x:v>
@@ -16003,10 +16318,13 @@
       <x:c r="AT107" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU107" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="108" spans="1:46">
+    <x:row r="108" spans="1:47">
       <x:c r="A108" s="3" t="s">
-        <x:v>151</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="B108" s="4" t="n">
         <x:v>6</x:v>
@@ -16143,10 +16461,13 @@
       <x:c r="AT108" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU108" s="4" t="n">
+        <x:v>3</x:v>
+      </x:c>
     </x:row>
-    <x:row r="109" spans="1:46">
+    <x:row r="109" spans="1:47">
       <x:c r="A109" s="3" t="s">
-        <x:v>152</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="B109" s="4" t="n">
         <x:v>0</x:v>
@@ -16283,10 +16604,13 @@
       <x:c r="AT109" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU109" s="4" t="n">
+        <x:v>1</x:v>
+      </x:c>
     </x:row>
-    <x:row r="110" spans="1:46">
+    <x:row r="110" spans="1:47">
       <x:c r="A110" s="3" t="s">
-        <x:v>153</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="B110" s="4" t="n">
         <x:v>2</x:v>
@@ -16423,10 +16747,13 @@
       <x:c r="AT110" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU110" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="111" spans="1:46">
+    <x:row r="111" spans="1:47">
       <x:c r="A111" s="3" t="s">
-        <x:v>154</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="B111" s="4" t="n">
         <x:v>12</x:v>
@@ -16563,10 +16890,13 @@
       <x:c r="AT111" s="4" t="n">
         <x:v>6</x:v>
       </x:c>
+      <x:c r="AU111" s="4" t="n">
+        <x:v>12</x:v>
+      </x:c>
     </x:row>
-    <x:row r="112" spans="1:46">
+    <x:row r="112" spans="1:47">
       <x:c r="A112" s="3" t="s">
-        <x:v>155</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="B112" s="4" t="n">
         <x:v>1</x:v>
@@ -16703,10 +17033,13 @@
       <x:c r="AT112" s="4" t="n">
         <x:v>7</x:v>
       </x:c>
+      <x:c r="AU112" s="4" t="n">
+        <x:v>5</x:v>
+      </x:c>
     </x:row>
-    <x:row r="113" spans="1:46">
+    <x:row r="113" spans="1:47">
       <x:c r="A113" s="3" t="s">
-        <x:v>156</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="B113" s="4" t="n">
         <x:v>2</x:v>
@@ -16843,10 +17176,13 @@
       <x:c r="AT113" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU113" s="4" t="n">
+        <x:v>4</x:v>
+      </x:c>
     </x:row>
-    <x:row r="114" spans="1:46">
+    <x:row r="114" spans="1:47">
       <x:c r="A114" s="3" t="s">
-        <x:v>157</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="B114" s="4" t="n">
         <x:v>3</x:v>
@@ -16983,10 +17319,13 @@
       <x:c r="AT114" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU114" s="4" t="n">
+        <x:v>1</x:v>
+      </x:c>
     </x:row>
-    <x:row r="115" spans="1:46">
+    <x:row r="115" spans="1:47">
       <x:c r="A115" s="3" t="s">
-        <x:v>158</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="B115" s="4" t="n">
         <x:v>0</x:v>
@@ -17123,10 +17462,13 @@
       <x:c r="AT115" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU115" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="116" spans="1:46">
+    <x:row r="116" spans="1:47">
       <x:c r="A116" s="3" t="s">
-        <x:v>159</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="B116" s="4" t="n">
         <x:v>3</x:v>
@@ -17263,10 +17605,13 @@
       <x:c r="AT116" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU116" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="117" spans="1:46">
+    <x:row r="117" spans="1:47">
       <x:c r="A117" s="3" t="s">
-        <x:v>160</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="B117" s="4" t="n">
         <x:v>72</x:v>
@@ -17403,10 +17748,13 @@
       <x:c r="AT117" s="4" t="n">
         <x:v>11</x:v>
       </x:c>
+      <x:c r="AU117" s="4" t="n">
+        <x:v>33</x:v>
+      </x:c>
     </x:row>
-    <x:row r="118" spans="1:46">
+    <x:row r="118" spans="1:47">
       <x:c r="A118" s="3" t="s">
-        <x:v>161</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="B118" s="4" t="n">
         <x:v>273</x:v>
@@ -17543,10 +17891,13 @@
       <x:c r="AT118" s="4" t="n">
         <x:v>73</x:v>
       </x:c>
+      <x:c r="AU118" s="4" t="n">
+        <x:v>108</x:v>
+      </x:c>
     </x:row>
-    <x:row r="119" spans="1:46">
+    <x:row r="119" spans="1:47">
       <x:c r="A119" s="3" t="s">
-        <x:v>162</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="B119" s="4" t="n">
         <x:v>0</x:v>
@@ -17683,10 +18034,13 @@
       <x:c r="AT119" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU119" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="120" spans="1:46">
+    <x:row r="120" spans="1:47">
       <x:c r="A120" s="3" t="s">
-        <x:v>163</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="B120" s="4" t="n">
         <x:v>0</x:v>
@@ -17823,10 +18177,13 @@
       <x:c r="AT120" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU120" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="121" spans="1:46">
+    <x:row r="121" spans="1:47">
       <x:c r="A121" s="3" t="s">
-        <x:v>164</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="B121" s="4" t="n">
         <x:v>16</x:v>
@@ -17963,10 +18320,13 @@
       <x:c r="AT121" s="4" t="n">
         <x:v>1</x:v>
       </x:c>
+      <x:c r="AU121" s="4" t="n">
+        <x:v>10</x:v>
+      </x:c>
     </x:row>
-    <x:row r="122" spans="1:46">
+    <x:row r="122" spans="1:47">
       <x:c r="A122" s="3" t="s">
-        <x:v>165</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="B122" s="4" t="n">
         <x:v>0</x:v>
@@ -18103,10 +18463,13 @@
       <x:c r="AT122" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU122" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="123" spans="1:46">
+    <x:row r="123" spans="1:47">
       <x:c r="A123" s="3" t="s">
-        <x:v>166</x:v>
+        <x:v>167</x:v>
       </x:c>
       <x:c r="B123" s="4" t="n">
         <x:v>0</x:v>
@@ -18243,10 +18606,13 @@
       <x:c r="AT123" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU123" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="124" spans="1:46">
+    <x:row r="124" spans="1:47">
       <x:c r="A124" s="3" t="s">
-        <x:v>167</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="B124" s="4" t="n">
         <x:v>0</x:v>
@@ -18383,10 +18749,13 @@
       <x:c r="AT124" s="4" t="n">
         <x:v>1</x:v>
       </x:c>
+      <x:c r="AU124" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="125" spans="1:46">
+    <x:row r="125" spans="1:47">
       <x:c r="A125" s="3" t="s">
-        <x:v>168</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="B125" s="4" t="n">
         <x:v>0</x:v>
@@ -18523,10 +18892,13 @@
       <x:c r="AT125" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU125" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="126" spans="1:46">
+    <x:row r="126" spans="1:47">
       <x:c r="A126" s="3" t="s">
-        <x:v>169</x:v>
+        <x:v>170</x:v>
       </x:c>
       <x:c r="B126" s="4" t="n">
         <x:v>3</x:v>
@@ -18663,10 +19035,13 @@
       <x:c r="AT126" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU126" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="127" spans="1:46">
+    <x:row r="127" spans="1:47">
       <x:c r="A127" s="3" t="s">
-        <x:v>170</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="B127" s="4" t="n">
         <x:v>2</x:v>
@@ -18803,10 +19178,13 @@
       <x:c r="AT127" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU127" s="4" t="n">
+        <x:v>1</x:v>
+      </x:c>
     </x:row>
-    <x:row r="128" spans="1:46">
+    <x:row r="128" spans="1:47">
       <x:c r="A128" s="3" t="s">
-        <x:v>171</x:v>
+        <x:v>172</x:v>
       </x:c>
       <x:c r="B128" s="4" t="n">
         <x:v>20</x:v>
@@ -18943,10 +19321,13 @@
       <x:c r="AT128" s="4" t="n">
         <x:v>12</x:v>
       </x:c>
+      <x:c r="AU128" s="4" t="n">
+        <x:v>24</x:v>
+      </x:c>
     </x:row>
-    <x:row r="129" spans="1:46">
+    <x:row r="129" spans="1:47">
       <x:c r="A129" s="3" t="s">
-        <x:v>172</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="B129" s="4" t="n">
         <x:v>0</x:v>
@@ -19083,10 +19464,13 @@
       <x:c r="AT129" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU129" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="130" spans="1:46">
+    <x:row r="130" spans="1:47">
       <x:c r="A130" s="3" t="s">
-        <x:v>173</x:v>
+        <x:v>174</x:v>
       </x:c>
       <x:c r="B130" s="4" t="n">
         <x:v>23</x:v>
@@ -19223,10 +19607,13 @@
       <x:c r="AT130" s="4" t="n">
         <x:v>3</x:v>
       </x:c>
+      <x:c r="AU130" s="4" t="n">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
-    <x:row r="131" spans="1:46">
+    <x:row r="131" spans="1:47">
       <x:c r="A131" s="3" t="s">
-        <x:v>174</x:v>
+        <x:v>175</x:v>
       </x:c>
       <x:c r="B131" s="4" t="n">
         <x:v>11</x:v>
@@ -19363,10 +19750,13 @@
       <x:c r="AT131" s="4" t="n">
         <x:v>5</x:v>
       </x:c>
+      <x:c r="AU131" s="4" t="n">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
-    <x:row r="132" spans="1:46">
+    <x:row r="132" spans="1:47">
       <x:c r="A132" s="3" t="s">
-        <x:v>175</x:v>
+        <x:v>176</x:v>
       </x:c>
       <x:c r="B132" s="4" t="n">
         <x:v>5</x:v>
@@ -19503,10 +19893,13 @@
       <x:c r="AT132" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU132" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="133" spans="1:46">
+    <x:row r="133" spans="1:47">
       <x:c r="A133" s="3" t="s">
-        <x:v>176</x:v>
+        <x:v>177</x:v>
       </x:c>
       <x:c r="B133" s="4" t="n">
         <x:v>0</x:v>
@@ -19643,10 +20036,13 @@
       <x:c r="AT133" s="4" t="n">
         <x:v>7</x:v>
       </x:c>
+      <x:c r="AU133" s="4" t="n">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
-    <x:row r="134" spans="1:46">
+    <x:row r="134" spans="1:47">
       <x:c r="A134" s="3" t="s">
-        <x:v>177</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="B134" s="4" t="n">
         <x:v>0</x:v>
@@ -19783,10 +20179,13 @@
       <x:c r="AT134" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU134" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="135" spans="1:46">
+    <x:row r="135" spans="1:47">
       <x:c r="A135" s="3" t="s">
-        <x:v>178</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="B135" s="4" t="n">
         <x:v>0</x:v>
@@ -19923,10 +20322,13 @@
       <x:c r="AT135" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU135" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="136" spans="1:46">
+    <x:row r="136" spans="1:47">
       <x:c r="A136" s="3" t="s">
-        <x:v>179</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="B136" s="4" t="n">
         <x:v>1</x:v>
@@ -20063,10 +20465,13 @@
       <x:c r="AT136" s="4" t="n">
         <x:v>1</x:v>
       </x:c>
+      <x:c r="AU136" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="137" spans="1:46">
+    <x:row r="137" spans="1:47">
       <x:c r="A137" s="3" t="s">
-        <x:v>180</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="B137" s="4" t="n">
         <x:v>13</x:v>
@@ -20203,10 +20608,13 @@
       <x:c r="AT137" s="4" t="n">
         <x:v>1</x:v>
       </x:c>
+      <x:c r="AU137" s="4" t="n">
+        <x:v>5</x:v>
+      </x:c>
     </x:row>
-    <x:row r="138" spans="1:46">
+    <x:row r="138" spans="1:47">
       <x:c r="A138" s="3" t="s">
-        <x:v>181</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="B138" s="4" t="n">
         <x:v>4</x:v>
@@ -20343,10 +20751,13 @@
       <x:c r="AT138" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU138" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="139" spans="1:46">
+    <x:row r="139" spans="1:47">
       <x:c r="A139" s="3" t="s">
-        <x:v>182</x:v>
+        <x:v>183</x:v>
       </x:c>
       <x:c r="B139" s="4" t="n">
         <x:v>0</x:v>
@@ -20483,10 +20894,13 @@
       <x:c r="AT139" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU139" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="140" spans="1:46">
+    <x:row r="140" spans="1:47">
       <x:c r="A140" s="3" t="s">
-        <x:v>183</x:v>
+        <x:v>184</x:v>
       </x:c>
       <x:c r="B140" s="4" t="n">
         <x:v>0</x:v>
@@ -20623,10 +21037,13 @@
       <x:c r="AT140" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU140" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="141" spans="1:46">
+    <x:row r="141" spans="1:47">
       <x:c r="A141" s="3" t="s">
-        <x:v>184</x:v>
+        <x:v>185</x:v>
       </x:c>
       <x:c r="B141" s="4" t="n">
         <x:v>0</x:v>
@@ -20763,10 +21180,13 @@
       <x:c r="AT141" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU141" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="142" spans="1:46">
+    <x:row r="142" spans="1:47">
       <x:c r="A142" s="3" t="s">
-        <x:v>185</x:v>
+        <x:v>186</x:v>
       </x:c>
       <x:c r="B142" s="4" t="n">
         <x:v>0</x:v>
@@ -20903,10 +21323,13 @@
       <x:c r="AT142" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU142" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="143" spans="1:46">
+    <x:row r="143" spans="1:47">
       <x:c r="A143" s="3" t="s">
-        <x:v>186</x:v>
+        <x:v>187</x:v>
       </x:c>
       <x:c r="B143" s="4" t="n">
         <x:v>0</x:v>
@@ -21043,10 +21466,13 @@
       <x:c r="AT143" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU143" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="144" spans="1:46">
+    <x:row r="144" spans="1:47">
       <x:c r="A144" s="3" t="s">
-        <x:v>187</x:v>
+        <x:v>188</x:v>
       </x:c>
       <x:c r="B144" s="4" t="n">
         <x:v>0</x:v>
@@ -21183,10 +21609,13 @@
       <x:c r="AT144" s="4" t="n">
         <x:v>1</x:v>
       </x:c>
+      <x:c r="AU144" s="4" t="n">
+        <x:v>3</x:v>
+      </x:c>
     </x:row>
-    <x:row r="145" spans="1:46">
+    <x:row r="145" spans="1:47">
       <x:c r="A145" s="3" t="s">
-        <x:v>188</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="B145" s="4" t="n">
         <x:v>0</x:v>
@@ -21323,10 +21752,13 @@
       <x:c r="AT145" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU145" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="146" spans="1:46">
+    <x:row r="146" spans="1:47">
       <x:c r="A146" s="3" t="s">
-        <x:v>189</x:v>
+        <x:v>190</x:v>
       </x:c>
       <x:c r="B146" s="4" t="n">
         <x:v>0</x:v>
@@ -21463,10 +21895,13 @@
       <x:c r="AT146" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU146" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="147" spans="1:46">
+    <x:row r="147" spans="1:47">
       <x:c r="A147" s="3" t="s">
-        <x:v>190</x:v>
+        <x:v>191</x:v>
       </x:c>
       <x:c r="B147" s="4" t="n">
         <x:v>0</x:v>
@@ -21603,10 +22038,13 @@
       <x:c r="AT147" s="4" t="n">
         <x:v>1</x:v>
       </x:c>
+      <x:c r="AU147" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="148" spans="1:46">
+    <x:row r="148" spans="1:47">
       <x:c r="A148" s="3" t="s">
-        <x:v>191</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="B148" s="4" t="n">
         <x:v>3</x:v>
@@ -21743,10 +22181,13 @@
       <x:c r="AT148" s="4" t="n">
         <x:v>1</x:v>
       </x:c>
+      <x:c r="AU148" s="4" t="n">
+        <x:v>2</x:v>
+      </x:c>
     </x:row>
-    <x:row r="149" spans="1:46">
+    <x:row r="149" spans="1:47">
       <x:c r="A149" s="3" t="s">
-        <x:v>192</x:v>
+        <x:v>193</x:v>
       </x:c>
       <x:c r="B149" s="4" t="n">
         <x:v>0</x:v>
@@ -21883,10 +22324,13 @@
       <x:c r="AT149" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU149" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="150" spans="1:46">
+    <x:row r="150" spans="1:47">
       <x:c r="A150" s="3" t="s">
-        <x:v>193</x:v>
+        <x:v>194</x:v>
       </x:c>
       <x:c r="B150" s="4" t="n">
         <x:v>6</x:v>
@@ -22023,10 +22467,13 @@
       <x:c r="AT150" s="4" t="n">
         <x:v>19</x:v>
       </x:c>
+      <x:c r="AU150" s="4" t="n">
+        <x:v>24</x:v>
+      </x:c>
     </x:row>
-    <x:row r="151" spans="1:46">
+    <x:row r="151" spans="1:47">
       <x:c r="A151" s="3" t="s">
-        <x:v>194</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="B151" s="4" t="n">
         <x:v>0</x:v>
@@ -22163,10 +22610,13 @@
       <x:c r="AT151" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU151" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="152" spans="1:46">
+    <x:row r="152" spans="1:47">
       <x:c r="A152" s="3" t="s">
-        <x:v>195</x:v>
+        <x:v>196</x:v>
       </x:c>
       <x:c r="B152" s="4" t="n">
         <x:v>0</x:v>
@@ -22303,10 +22753,13 @@
       <x:c r="AT152" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU152" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="153" spans="1:46">
+    <x:row r="153" spans="1:47">
       <x:c r="A153" s="3" t="s">
-        <x:v>196</x:v>
+        <x:v>197</x:v>
       </x:c>
       <x:c r="B153" s="4" t="n">
         <x:v>2</x:v>
@@ -22443,10 +22896,13 @@
       <x:c r="AT153" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU153" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="154" spans="1:46">
+    <x:row r="154" spans="1:47">
       <x:c r="A154" s="3" t="s">
-        <x:v>197</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="B154" s="4" t="n">
         <x:v>2</x:v>
@@ -22583,10 +23039,13 @@
       <x:c r="AT154" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU154" s="4" t="n">
+        <x:v>1</x:v>
+      </x:c>
     </x:row>
-    <x:row r="155" spans="1:46">
+    <x:row r="155" spans="1:47">
       <x:c r="A155" s="3" t="s">
-        <x:v>198</x:v>
+        <x:v>199</x:v>
       </x:c>
       <x:c r="B155" s="4" t="n">
         <x:v>1</x:v>
@@ -22723,10 +23182,13 @@
       <x:c r="AT155" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU155" s="4" t="n">
+        <x:v>1</x:v>
+      </x:c>
     </x:row>
-    <x:row r="156" spans="1:46">
+    <x:row r="156" spans="1:47">
       <x:c r="A156" s="3" t="s">
-        <x:v>199</x:v>
+        <x:v>200</x:v>
       </x:c>
       <x:c r="B156" s="4" t="n">
         <x:v>8</x:v>
@@ -22863,10 +23325,13 @@
       <x:c r="AT156" s="4" t="n">
         <x:v>4</x:v>
       </x:c>
+      <x:c r="AU156" s="4" t="n">
+        <x:v>3</x:v>
+      </x:c>
     </x:row>
-    <x:row r="157" spans="1:46">
+    <x:row r="157" spans="1:47">
       <x:c r="A157" s="3" t="s">
-        <x:v>200</x:v>
+        <x:v>201</x:v>
       </x:c>
       <x:c r="B157" s="4" t="n">
         <x:v>0</x:v>
@@ -23003,10 +23468,13 @@
       <x:c r="AT157" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU157" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="158" spans="1:46">
+    <x:row r="158" spans="1:47">
       <x:c r="A158" s="3" t="s">
-        <x:v>201</x:v>
+        <x:v>202</x:v>
       </x:c>
       <x:c r="B158" s="4" t="n">
         <x:v>0</x:v>
@@ -23143,10 +23611,13 @@
       <x:c r="AT158" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU158" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="159" spans="1:46">
+    <x:row r="159" spans="1:47">
       <x:c r="A159" s="3" t="s">
-        <x:v>202</x:v>
+        <x:v>203</x:v>
       </x:c>
       <x:c r="B159" s="4" t="n">
         <x:v>0</x:v>
@@ -23283,10 +23754,13 @@
       <x:c r="AT159" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU159" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="160" spans="1:46">
+    <x:row r="160" spans="1:47">
       <x:c r="A160" s="3" t="s">
-        <x:v>203</x:v>
+        <x:v>204</x:v>
       </x:c>
       <x:c r="B160" s="4" t="n">
         <x:v>0</x:v>
@@ -23423,10 +23897,13 @@
       <x:c r="AT160" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU160" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="161" spans="1:46">
+    <x:row r="161" spans="1:47">
       <x:c r="A161" s="3" t="s">
-        <x:v>204</x:v>
+        <x:v>205</x:v>
       </x:c>
       <x:c r="B161" s="4" t="n">
         <x:v>0</x:v>
@@ -23563,10 +24040,13 @@
       <x:c r="AT161" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU161" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="162" spans="1:46">
+    <x:row r="162" spans="1:47">
       <x:c r="A162" s="3" t="s">
-        <x:v>205</x:v>
+        <x:v>206</x:v>
       </x:c>
       <x:c r="B162" s="4" t="n">
         <x:v>4</x:v>
@@ -23703,10 +24183,13 @@
       <x:c r="AT162" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU162" s="4" t="n">
+        <x:v>2</x:v>
+      </x:c>
     </x:row>
-    <x:row r="163" spans="1:46">
+    <x:row r="163" spans="1:47">
       <x:c r="A163" s="3" t="s">
-        <x:v>206</x:v>
+        <x:v>207</x:v>
       </x:c>
       <x:c r="B163" s="4" t="n">
         <x:v>13</x:v>
@@ -23843,10 +24326,13 @@
       <x:c r="AT163" s="4" t="n">
         <x:v>1</x:v>
       </x:c>
+      <x:c r="AU163" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="164" spans="1:46">
+    <x:row r="164" spans="1:47">
       <x:c r="A164" s="3" t="s">
-        <x:v>207</x:v>
+        <x:v>208</x:v>
       </x:c>
       <x:c r="B164" s="4" t="n">
         <x:v>5</x:v>
@@ -23983,10 +24469,13 @@
       <x:c r="AT164" s="4" t="n">
         <x:v>4</x:v>
       </x:c>
+      <x:c r="AU164" s="4" t="n">
+        <x:v>17</x:v>
+      </x:c>
     </x:row>
-    <x:row r="165" spans="1:46">
+    <x:row r="165" spans="1:47">
       <x:c r="A165" s="3" t="s">
-        <x:v>208</x:v>
+        <x:v>209</x:v>
       </x:c>
       <x:c r="B165" s="4" t="n">
         <x:v>0</x:v>
@@ -24123,10 +24612,13 @@
       <x:c r="AT165" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU165" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="166" spans="1:46">
+    <x:row r="166" spans="1:47">
       <x:c r="A166" s="3" t="s">
-        <x:v>209</x:v>
+        <x:v>210</x:v>
       </x:c>
       <x:c r="B166" s="4" t="n">
         <x:v>0</x:v>
@@ -24263,10 +24755,13 @@
       <x:c r="AT166" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU166" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="167" spans="1:46">
+    <x:row r="167" spans="1:47">
       <x:c r="A167" s="3" t="s">
-        <x:v>210</x:v>
+        <x:v>211</x:v>
       </x:c>
       <x:c r="B167" s="4" t="n">
         <x:v>0</x:v>
@@ -24403,10 +24898,13 @@
       <x:c r="AT167" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU167" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="168" spans="1:46">
+    <x:row r="168" spans="1:47">
       <x:c r="A168" s="3" t="s">
-        <x:v>211</x:v>
+        <x:v>212</x:v>
       </x:c>
       <x:c r="B168" s="4" t="n">
         <x:v>2</x:v>
@@ -24543,10 +25041,13 @@
       <x:c r="AT168" s="4" t="n">
         <x:v>83</x:v>
       </x:c>
+      <x:c r="AU168" s="4" t="n">
+        <x:v>149</x:v>
+      </x:c>
     </x:row>
-    <x:row r="169" spans="1:46">
+    <x:row r="169" spans="1:47">
       <x:c r="A169" s="3" t="s">
-        <x:v>212</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="B169" s="4" t="n">
         <x:v>0</x:v>
@@ -24683,10 +25184,13 @@
       <x:c r="AT169" s="4" t="n">
         <x:v>5</x:v>
       </x:c>
+      <x:c r="AU169" s="4" t="n">
+        <x:v>12</x:v>
+      </x:c>
     </x:row>
-    <x:row r="170" spans="1:46">
+    <x:row r="170" spans="1:47">
       <x:c r="A170" s="3" t="s">
-        <x:v>213</x:v>
+        <x:v>214</x:v>
       </x:c>
       <x:c r="B170" s="4" t="n">
         <x:v>0</x:v>
@@ -24823,10 +25327,13 @@
       <x:c r="AT170" s="4" t="n">
         <x:v>3</x:v>
       </x:c>
+      <x:c r="AU170" s="4" t="n">
+        <x:v>5</x:v>
+      </x:c>
     </x:row>
-    <x:row r="171" spans="1:46">
+    <x:row r="171" spans="1:47">
       <x:c r="A171" s="3" t="s">
-        <x:v>214</x:v>
+        <x:v>215</x:v>
       </x:c>
       <x:c r="B171" s="4" t="n">
         <x:v>2</x:v>
@@ -24963,10 +25470,13 @@
       <x:c r="AT171" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU171" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="172" spans="1:46">
+    <x:row r="172" spans="1:47">
       <x:c r="A172" s="3" t="s">
-        <x:v>215</x:v>
+        <x:v>216</x:v>
       </x:c>
       <x:c r="B172" s="4" t="n">
         <x:v>49</x:v>
@@ -25103,10 +25613,13 @@
       <x:c r="AT172" s="4" t="n">
         <x:v>57</x:v>
       </x:c>
+      <x:c r="AU172" s="4" t="n">
+        <x:v>73</x:v>
+      </x:c>
     </x:row>
-    <x:row r="173" spans="1:46">
+    <x:row r="173" spans="1:47">
       <x:c r="A173" s="3" t="s">
-        <x:v>216</x:v>
+        <x:v>217</x:v>
       </x:c>
       <x:c r="B173" s="4" t="n">
         <x:v>0</x:v>
@@ -25243,10 +25756,13 @@
       <x:c r="AT173" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU173" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="174" spans="1:46">
+    <x:row r="174" spans="1:47">
       <x:c r="A174" s="3" t="s">
-        <x:v>217</x:v>
+        <x:v>218</x:v>
       </x:c>
       <x:c r="B174" s="4" t="n">
         <x:v>0</x:v>
@@ -25383,10 +25899,13 @@
       <x:c r="AT174" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU174" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="175" spans="1:46">
+    <x:row r="175" spans="1:47">
       <x:c r="A175" s="3" t="s">
-        <x:v>218</x:v>
+        <x:v>219</x:v>
       </x:c>
       <x:c r="B175" s="4" t="n">
         <x:v>3</x:v>
@@ -25523,10 +26042,13 @@
       <x:c r="AT175" s="4" t="n">
         <x:v>4</x:v>
       </x:c>
+      <x:c r="AU175" s="4" t="n">
+        <x:v>3</x:v>
+      </x:c>
     </x:row>
-    <x:row r="176" spans="1:46">
+    <x:row r="176" spans="1:47">
       <x:c r="A176" s="3" t="s">
-        <x:v>219</x:v>
+        <x:v>220</x:v>
       </x:c>
       <x:c r="B176" s="4" t="n">
         <x:v>0</x:v>
@@ -25663,10 +26185,13 @@
       <x:c r="AT176" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU176" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="177" spans="1:46">
+    <x:row r="177" spans="1:47">
       <x:c r="A177" s="3" t="s">
-        <x:v>220</x:v>
+        <x:v>221</x:v>
       </x:c>
       <x:c r="B177" s="4" t="n">
         <x:v>36</x:v>
@@ -25803,10 +26328,13 @@
       <x:c r="AT177" s="4" t="n">
         <x:v>38</x:v>
       </x:c>
+      <x:c r="AU177" s="4" t="n">
+        <x:v>80</x:v>
+      </x:c>
     </x:row>
-    <x:row r="178" spans="1:46">
+    <x:row r="178" spans="1:47">
       <x:c r="A178" s="3" t="s">
-        <x:v>221</x:v>
+        <x:v>222</x:v>
       </x:c>
       <x:c r="B178" s="4" t="n">
         <x:v>0</x:v>
@@ -25943,10 +26471,13 @@
       <x:c r="AT178" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU178" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="179" spans="1:46">
+    <x:row r="179" spans="1:47">
       <x:c r="A179" s="3" t="s">
-        <x:v>222</x:v>
+        <x:v>223</x:v>
       </x:c>
       <x:c r="B179" s="4" t="n">
         <x:v>0</x:v>
@@ -26083,10 +26614,13 @@
       <x:c r="AT179" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU179" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="180" spans="1:46">
+    <x:row r="180" spans="1:47">
       <x:c r="A180" s="3" t="s">
-        <x:v>223</x:v>
+        <x:v>224</x:v>
       </x:c>
       <x:c r="B180" s="4" t="n">
         <x:v>0</x:v>
@@ -26223,10 +26757,13 @@
       <x:c r="AT180" s="4" t="n">
         <x:v>3</x:v>
       </x:c>
+      <x:c r="AU180" s="4" t="n">
+        <x:v>3</x:v>
+      </x:c>
     </x:row>
-    <x:row r="181" spans="1:46">
+    <x:row r="181" spans="1:47">
       <x:c r="A181" s="3" t="s">
-        <x:v>224</x:v>
+        <x:v>225</x:v>
       </x:c>
       <x:c r="B181" s="4" t="n">
         <x:v>3</x:v>
@@ -26363,10 +26900,13 @@
       <x:c r="AT181" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU181" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="182" spans="1:46">
+    <x:row r="182" spans="1:47">
       <x:c r="A182" s="3" t="s">
-        <x:v>225</x:v>
+        <x:v>226</x:v>
       </x:c>
       <x:c r="B182" s="4" t="n">
         <x:v>175</x:v>
@@ -26503,10 +27043,13 @@
       <x:c r="AT182" s="4" t="n">
         <x:v>130</x:v>
       </x:c>
+      <x:c r="AU182" s="4" t="n">
+        <x:v>300</x:v>
+      </x:c>
     </x:row>
-    <x:row r="183" spans="1:46">
+    <x:row r="183" spans="1:47">
       <x:c r="A183" s="3" t="s">
-        <x:v>226</x:v>
+        <x:v>227</x:v>
       </x:c>
       <x:c r="B183" s="4" t="n">
         <x:v>0</x:v>
@@ -26643,10 +27186,13 @@
       <x:c r="AT183" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU183" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="184" spans="1:46">
+    <x:row r="184" spans="1:47">
       <x:c r="A184" s="3" t="s">
-        <x:v>227</x:v>
+        <x:v>228</x:v>
       </x:c>
       <x:c r="B184" s="4" t="n">
         <x:v>17</x:v>
@@ -26783,10 +27329,13 @@
       <x:c r="AT184" s="4" t="n">
         <x:v>4</x:v>
       </x:c>
+      <x:c r="AU184" s="4" t="n">
+        <x:v>6</x:v>
+      </x:c>
     </x:row>
-    <x:row r="185" spans="1:46">
+    <x:row r="185" spans="1:47">
       <x:c r="A185" s="3" t="s">
-        <x:v>228</x:v>
+        <x:v>229</x:v>
       </x:c>
       <x:c r="B185" s="4" t="n">
         <x:v>14</x:v>
@@ -26923,10 +27472,13 @@
       <x:c r="AT185" s="4" t="n">
         <x:v>85</x:v>
       </x:c>
+      <x:c r="AU185" s="4" t="n">
+        <x:v>119</x:v>
+      </x:c>
     </x:row>
-    <x:row r="186" spans="1:46">
+    <x:row r="186" spans="1:47">
       <x:c r="A186" s="3" t="s">
-        <x:v>229</x:v>
+        <x:v>230</x:v>
       </x:c>
       <x:c r="B186" s="4" t="n">
         <x:v>71</x:v>
@@ -27063,10 +27615,13 @@
       <x:c r="AT186" s="4" t="n">
         <x:v>113</x:v>
       </x:c>
+      <x:c r="AU186" s="4" t="n">
+        <x:v>286</x:v>
+      </x:c>
     </x:row>
-    <x:row r="187" spans="1:46">
+    <x:row r="187" spans="1:47">
       <x:c r="A187" s="3" t="s">
-        <x:v>230</x:v>
+        <x:v>231</x:v>
       </x:c>
       <x:c r="B187" s="4" t="n">
         <x:v>137</x:v>
@@ -27203,10 +27758,13 @@
       <x:c r="AT187" s="4" t="n">
         <x:v>2</x:v>
       </x:c>
+      <x:c r="AU187" s="4" t="n">
+        <x:v>12</x:v>
+      </x:c>
     </x:row>
-    <x:row r="188" spans="1:46">
+    <x:row r="188" spans="1:47">
       <x:c r="A188" s="3" t="s">
-        <x:v>231</x:v>
+        <x:v>232</x:v>
       </x:c>
       <x:c r="B188" s="4" t="n">
         <x:v>29</x:v>
@@ -27343,10 +27901,13 @@
       <x:c r="AT188" s="4" t="n">
         <x:v>1</x:v>
       </x:c>
+      <x:c r="AU188" s="4" t="n">
+        <x:v>5</x:v>
+      </x:c>
     </x:row>
-    <x:row r="189" spans="1:46">
+    <x:row r="189" spans="1:47">
       <x:c r="A189" s="3" t="s">
-        <x:v>232</x:v>
+        <x:v>233</x:v>
       </x:c>
       <x:c r="B189" s="4" t="n">
         <x:v>17</x:v>
@@ -27483,10 +28044,13 @@
       <x:c r="AT189" s="4" t="n">
         <x:v>12</x:v>
       </x:c>
+      <x:c r="AU189" s="4" t="n">
+        <x:v>7</x:v>
+      </x:c>
     </x:row>
-    <x:row r="190" spans="1:46">
+    <x:row r="190" spans="1:47">
       <x:c r="A190" s="3" t="s">
-        <x:v>233</x:v>
+        <x:v>234</x:v>
       </x:c>
       <x:c r="B190" s="4" t="n">
         <x:v>0</x:v>
@@ -27623,10 +28187,13 @@
       <x:c r="AT190" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU190" s="4" t="n">
+        <x:v>4</x:v>
+      </x:c>
     </x:row>
-    <x:row r="191" spans="1:46">
+    <x:row r="191" spans="1:47">
       <x:c r="A191" s="3" t="s">
-        <x:v>234</x:v>
+        <x:v>235</x:v>
       </x:c>
       <x:c r="B191" s="4" t="n">
         <x:v>8</x:v>
@@ -27763,10 +28330,13 @@
       <x:c r="AT191" s="4" t="n">
         <x:v>40</x:v>
       </x:c>
+      <x:c r="AU191" s="4" t="n">
+        <x:v>92</x:v>
+      </x:c>
     </x:row>
-    <x:row r="192" spans="1:46">
+    <x:row r="192" spans="1:47">
       <x:c r="A192" s="3" t="s">
-        <x:v>235</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="B192" s="4" t="n">
         <x:v>0</x:v>
@@ -27903,10 +28473,13 @@
       <x:c r="AT192" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU192" s="4" t="n">
+        <x:v>2</x:v>
+      </x:c>
     </x:row>
-    <x:row r="193" spans="1:46">
+    <x:row r="193" spans="1:47">
       <x:c r="A193" s="3" t="s">
-        <x:v>236</x:v>
+        <x:v>237</x:v>
       </x:c>
       <x:c r="B193" s="4" t="n">
         <x:v>0</x:v>
@@ -28043,10 +28616,13 @@
       <x:c r="AT193" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU193" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="194" spans="1:46">
+    <x:row r="194" spans="1:47">
       <x:c r="A194" s="3" t="s">
-        <x:v>237</x:v>
+        <x:v>238</x:v>
       </x:c>
       <x:c r="B194" s="4" t="n">
         <x:v>0</x:v>
@@ -28183,10 +28759,13 @@
       <x:c r="AT194" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU194" s="4" t="n">
+        <x:v>1</x:v>
+      </x:c>
     </x:row>
-    <x:row r="195" spans="1:46">
+    <x:row r="195" spans="1:47">
       <x:c r="A195" s="3" t="s">
-        <x:v>238</x:v>
+        <x:v>239</x:v>
       </x:c>
       <x:c r="B195" s="4" t="n">
         <x:v>56</x:v>
@@ -28323,10 +28902,13 @@
       <x:c r="AT195" s="4" t="n">
         <x:v>6</x:v>
       </x:c>
+      <x:c r="AU195" s="4" t="n">
+        <x:v>7</x:v>
+      </x:c>
     </x:row>
-    <x:row r="196" spans="1:46">
+    <x:row r="196" spans="1:47">
       <x:c r="A196" s="3" t="s">
-        <x:v>239</x:v>
+        <x:v>240</x:v>
       </x:c>
       <x:c r="B196" s="4" t="n">
         <x:v>0</x:v>
@@ -28463,10 +29045,13 @@
       <x:c r="AT196" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU196" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="197" spans="1:46">
+    <x:row r="197" spans="1:47">
       <x:c r="A197" s="3" t="s">
-        <x:v>240</x:v>
+        <x:v>241</x:v>
       </x:c>
       <x:c r="B197" s="4" t="n">
         <x:v>11</x:v>
@@ -28603,10 +29188,13 @@
       <x:c r="AT197" s="4" t="n">
         <x:v>1</x:v>
       </x:c>
+      <x:c r="AU197" s="4" t="n">
+        <x:v>2</x:v>
+      </x:c>
     </x:row>
-    <x:row r="198" spans="1:46">
+    <x:row r="198" spans="1:47">
       <x:c r="A198" s="3" t="s">
-        <x:v>241</x:v>
+        <x:v>242</x:v>
       </x:c>
       <x:c r="B198" s="4" t="n">
         <x:v>0</x:v>
@@ -28743,10 +29331,13 @@
       <x:c r="AT198" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU198" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="199" spans="1:46">
+    <x:row r="199" spans="1:47">
       <x:c r="A199" s="3" t="s">
-        <x:v>242</x:v>
+        <x:v>243</x:v>
       </x:c>
       <x:c r="B199" s="4" t="n">
         <x:v>0</x:v>
@@ -28883,10 +29474,13 @@
       <x:c r="AT199" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU199" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="200" spans="1:46">
+    <x:row r="200" spans="1:47">
       <x:c r="A200" s="3" t="s">
-        <x:v>243</x:v>
+        <x:v>244</x:v>
       </x:c>
       <x:c r="B200" s="4" t="n">
         <x:v>0</x:v>
@@ -29023,10 +29617,13 @@
       <x:c r="AT200" s="4" t="n">
         <x:v>1</x:v>
       </x:c>
+      <x:c r="AU200" s="4" t="n">
+        <x:v>1</x:v>
+      </x:c>
     </x:row>
-    <x:row r="201" spans="1:46">
+    <x:row r="201" spans="1:47">
       <x:c r="A201" s="3" t="s">
-        <x:v>244</x:v>
+        <x:v>245</x:v>
       </x:c>
       <x:c r="B201" s="4" t="n">
         <x:v>0</x:v>
@@ -29163,10 +29760,13 @@
       <x:c r="AT201" s="4" t="n">
         <x:v>16</x:v>
       </x:c>
+      <x:c r="AU201" s="4" t="n">
+        <x:v>27</x:v>
+      </x:c>
     </x:row>
-    <x:row r="202" spans="1:46">
+    <x:row r="202" spans="1:47">
       <x:c r="A202" s="3" t="s">
-        <x:v>245</x:v>
+        <x:v>246</x:v>
       </x:c>
       <x:c r="B202" s="4" t="n">
         <x:v>1</x:v>
@@ -29303,10 +29903,13 @@
       <x:c r="AT202" s="4" t="n">
         <x:v>82</x:v>
       </x:c>
+      <x:c r="AU202" s="4" t="n">
+        <x:v>114</x:v>
+      </x:c>
     </x:row>
-    <x:row r="203" spans="1:46">
+    <x:row r="203" spans="1:47">
       <x:c r="A203" s="3" t="s">
-        <x:v>246</x:v>
+        <x:v>247</x:v>
       </x:c>
       <x:c r="B203" s="4" t="n">
         <x:v>9</x:v>
@@ -29443,10 +30046,13 @@
       <x:c r="AT203" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU203" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="204" spans="1:46">
+    <x:row r="204" spans="1:47">
       <x:c r="A204" s="3" t="s">
-        <x:v>247</x:v>
+        <x:v>248</x:v>
       </x:c>
       <x:c r="B204" s="4" t="n">
         <x:v>7</x:v>
@@ -29583,10 +30189,13 @@
       <x:c r="AT204" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU204" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="205" spans="1:46">
+    <x:row r="205" spans="1:47">
       <x:c r="A205" s="3" t="s">
-        <x:v>248</x:v>
+        <x:v>249</x:v>
       </x:c>
       <x:c r="B205" s="4" t="n">
         <x:v>0</x:v>
@@ -29723,10 +30332,13 @@
       <x:c r="AT205" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU205" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="206" spans="1:46">
+    <x:row r="206" spans="1:47">
       <x:c r="A206" s="3" t="s">
-        <x:v>249</x:v>
+        <x:v>250</x:v>
       </x:c>
       <x:c r="B206" s="4" t="n">
         <x:v>172</x:v>
@@ -29863,10 +30475,13 @@
       <x:c r="AT206" s="4" t="n">
         <x:v>213</x:v>
       </x:c>
+      <x:c r="AU206" s="4" t="n">
+        <x:v>344</x:v>
+      </x:c>
     </x:row>
-    <x:row r="207" spans="1:46">
+    <x:row r="207" spans="1:47">
       <x:c r="A207" s="3" t="s">
-        <x:v>250</x:v>
+        <x:v>251</x:v>
       </x:c>
       <x:c r="B207" s="4" t="n">
         <x:v>0</x:v>
@@ -30003,10 +30618,13 @@
       <x:c r="AT207" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU207" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="208" spans="1:46">
+    <x:row r="208" spans="1:47">
       <x:c r="A208" s="3" t="s">
-        <x:v>251</x:v>
+        <x:v>252</x:v>
       </x:c>
       <x:c r="B208" s="4" t="n">
         <x:v>0</x:v>
@@ -30143,10 +30761,13 @@
       <x:c r="AT208" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU208" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="209" spans="1:46">
+    <x:row r="209" spans="1:47">
       <x:c r="A209" s="3" t="s">
-        <x:v>252</x:v>
+        <x:v>253</x:v>
       </x:c>
       <x:c r="B209" s="4" t="n">
         <x:v>4</x:v>
@@ -30283,10 +30904,13 @@
       <x:c r="AT209" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU209" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="210" spans="1:46">
+    <x:row r="210" spans="1:47">
       <x:c r="A210" s="3" t="s">
-        <x:v>253</x:v>
+        <x:v>254</x:v>
       </x:c>
       <x:c r="B210" s="4" t="n">
         <x:v>0</x:v>
@@ -30423,10 +31047,13 @@
       <x:c r="AT210" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU210" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="211" spans="1:46">
+    <x:row r="211" spans="1:47">
       <x:c r="A211" s="3" t="s">
-        <x:v>254</x:v>
+        <x:v>255</x:v>
       </x:c>
       <x:c r="B211" s="4" t="n">
         <x:v>12</x:v>
@@ -30563,10 +31190,13 @@
       <x:c r="AT211" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU211" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="212" spans="1:46">
+    <x:row r="212" spans="1:47">
       <x:c r="A212" s="3" t="s">
-        <x:v>255</x:v>
+        <x:v>256</x:v>
       </x:c>
       <x:c r="B212" s="4" t="n">
         <x:v>67</x:v>
@@ -30703,10 +31333,13 @@
       <x:c r="AT212" s="4" t="n">
         <x:v>14</x:v>
       </x:c>
+      <x:c r="AU212" s="4" t="n">
+        <x:v>30</x:v>
+      </x:c>
     </x:row>
-    <x:row r="213" spans="1:46">
+    <x:row r="213" spans="1:47">
       <x:c r="A213" s="3" t="s">
-        <x:v>256</x:v>
+        <x:v>257</x:v>
       </x:c>
       <x:c r="B213" s="4" t="n">
         <x:v>527</x:v>
@@ -30843,10 +31476,13 @@
       <x:c r="AT213" s="4" t="n">
         <x:v>3</x:v>
       </x:c>
+      <x:c r="AU213" s="4" t="n">
+        <x:v>3</x:v>
+      </x:c>
     </x:row>
-    <x:row r="214" spans="1:46">
+    <x:row r="214" spans="1:47">
       <x:c r="A214" s="3" t="s">
-        <x:v>257</x:v>
+        <x:v>258</x:v>
       </x:c>
       <x:c r="B214" s="4" t="n">
         <x:v>29</x:v>
@@ -30983,10 +31619,13 @@
       <x:c r="AT214" s="4" t="n">
         <x:v>26</x:v>
       </x:c>
+      <x:c r="AU214" s="4" t="n">
+        <x:v>255</x:v>
+      </x:c>
     </x:row>
-    <x:row r="215" spans="1:46">
+    <x:row r="215" spans="1:47">
       <x:c r="A215" s="3" t="s">
-        <x:v>258</x:v>
+        <x:v>259</x:v>
       </x:c>
       <x:c r="B215" s="4" t="n">
         <x:v>0</x:v>
@@ -31123,10 +31762,13 @@
       <x:c r="AT215" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU215" s="4" t="n">
+        <x:v>1</x:v>
+      </x:c>
     </x:row>
-    <x:row r="216" spans="1:46">
+    <x:row r="216" spans="1:47">
       <x:c r="A216" s="3" t="s">
-        <x:v>259</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="B216" s="4" t="n">
         <x:v>1</x:v>
@@ -31263,10 +31905,13 @@
       <x:c r="AT216" s="4" t="n">
         <x:v>1</x:v>
       </x:c>
+      <x:c r="AU216" s="4" t="n">
+        <x:v>11</x:v>
+      </x:c>
     </x:row>
-    <x:row r="217" spans="1:46">
+    <x:row r="217" spans="1:47">
       <x:c r="A217" s="3" t="s">
-        <x:v>260</x:v>
+        <x:v>261</x:v>
       </x:c>
       <x:c r="B217" s="4" t="n">
         <x:v>18</x:v>
@@ -31403,10 +32048,13 @@
       <x:c r="AT217" s="4" t="n">
         <x:v>69</x:v>
       </x:c>
+      <x:c r="AU217" s="4" t="n">
+        <x:v>104</x:v>
+      </x:c>
     </x:row>
-    <x:row r="218" spans="1:46">
+    <x:row r="218" spans="1:47">
       <x:c r="A218" s="3" t="s">
-        <x:v>261</x:v>
+        <x:v>262</x:v>
       </x:c>
       <x:c r="B218" s="4" t="n">
         <x:v>0</x:v>
@@ -31543,10 +32191,13 @@
       <x:c r="AT218" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU218" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="219" spans="1:46">
+    <x:row r="219" spans="1:47">
       <x:c r="A219" s="3" t="s">
-        <x:v>262</x:v>
+        <x:v>263</x:v>
       </x:c>
       <x:c r="B219" s="4" t="n">
         <x:v>0</x:v>
@@ -31683,10 +32334,13 @@
       <x:c r="AT219" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU219" s="4" t="n">
+        <x:v>1</x:v>
+      </x:c>
     </x:row>
-    <x:row r="220" spans="1:46">
+    <x:row r="220" spans="1:47">
       <x:c r="A220" s="3" t="s">
-        <x:v>263</x:v>
+        <x:v>264</x:v>
       </x:c>
       <x:c r="B220" s="4" t="n">
         <x:v>0</x:v>
@@ -31823,10 +32477,13 @@
       <x:c r="AT220" s="4" t="n">
         <x:v>3</x:v>
       </x:c>
+      <x:c r="AU220" s="4" t="n">
+        <x:v>30</x:v>
+      </x:c>
     </x:row>
-    <x:row r="221" spans="1:46">
+    <x:row r="221" spans="1:47">
       <x:c r="A221" s="3" t="s">
-        <x:v>264</x:v>
+        <x:v>265</x:v>
       </x:c>
       <x:c r="B221" s="4" t="n">
         <x:v>0</x:v>
@@ -31963,10 +32620,13 @@
       <x:c r="AT221" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU221" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="222" spans="1:46">
+    <x:row r="222" spans="1:47">
       <x:c r="A222" s="3" t="s">
-        <x:v>265</x:v>
+        <x:v>266</x:v>
       </x:c>
       <x:c r="B222" s="4" t="n">
         <x:v>3</x:v>
@@ -32103,10 +32763,13 @@
       <x:c r="AT222" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU222" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="223" spans="1:46">
+    <x:row r="223" spans="1:47">
       <x:c r="A223" s="3" t="s">
-        <x:v>266</x:v>
+        <x:v>267</x:v>
       </x:c>
       <x:c r="B223" s="4" t="n">
         <x:v>2</x:v>
@@ -32243,10 +32906,13 @@
       <x:c r="AT223" s="4" t="n">
         <x:v>38</x:v>
       </x:c>
+      <x:c r="AU223" s="4" t="n">
+        <x:v>68</x:v>
+      </x:c>
     </x:row>
-    <x:row r="224" spans="1:46">
+    <x:row r="224" spans="1:47">
       <x:c r="A224" s="3" t="s">
-        <x:v>267</x:v>
+        <x:v>268</x:v>
       </x:c>
       <x:c r="B224" s="4" t="n">
         <x:v>0</x:v>
@@ -32383,10 +33049,13 @@
       <x:c r="AT224" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU224" s="4" t="n">
+        <x:v>1</x:v>
+      </x:c>
     </x:row>
-    <x:row r="225" spans="1:46">
+    <x:row r="225" spans="1:47">
       <x:c r="A225" s="3" t="s">
-        <x:v>268</x:v>
+        <x:v>269</x:v>
       </x:c>
       <x:c r="B225" s="4" t="n">
         <x:v>0</x:v>
@@ -32523,10 +33192,13 @@
       <x:c r="AT225" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU225" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="226" spans="1:46">
+    <x:row r="226" spans="1:47">
       <x:c r="A226" s="3" t="s">
-        <x:v>269</x:v>
+        <x:v>270</x:v>
       </x:c>
       <x:c r="B226" s="4" t="n">
         <x:v>0</x:v>
@@ -32663,10 +33335,13 @@
       <x:c r="AT226" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU226" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="227" spans="1:46">
+    <x:row r="227" spans="1:47">
       <x:c r="A227" s="3" t="s">
-        <x:v>270</x:v>
+        <x:v>271</x:v>
       </x:c>
       <x:c r="B227" s="4" t="n">
         <x:v>40</x:v>
@@ -32803,10 +33478,13 @@
       <x:c r="AT227" s="4" t="n">
         <x:v>12</x:v>
       </x:c>
+      <x:c r="AU227" s="4" t="n">
+        <x:v>18</x:v>
+      </x:c>
     </x:row>
-    <x:row r="228" spans="1:46">
+    <x:row r="228" spans="1:47">
       <x:c r="A228" s="3" t="s">
-        <x:v>271</x:v>
+        <x:v>272</x:v>
       </x:c>
       <x:c r="B228" s="4" t="n">
         <x:v>0</x:v>
@@ -32943,10 +33621,13 @@
       <x:c r="AT228" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU228" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="229" spans="1:46">
+    <x:row r="229" spans="1:47">
       <x:c r="A229" s="3" t="s">
-        <x:v>272</x:v>
+        <x:v>273</x:v>
       </x:c>
       <x:c r="B229" s="4" t="n">
         <x:v>0</x:v>
@@ -33083,10 +33764,13 @@
       <x:c r="AT229" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU229" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="230" spans="1:46">
+    <x:row r="230" spans="1:47">
       <x:c r="A230" s="3" t="s">
-        <x:v>273</x:v>
+        <x:v>274</x:v>
       </x:c>
       <x:c r="B230" s="4" t="n">
         <x:v>0</x:v>
@@ -33223,10 +33907,13 @@
       <x:c r="AT230" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU230" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="231" spans="1:46">
+    <x:row r="231" spans="1:47">
       <x:c r="A231" s="3" t="s">
-        <x:v>274</x:v>
+        <x:v>275</x:v>
       </x:c>
       <x:c r="B231" s="4" t="n">
         <x:v>0</x:v>
@@ -33363,10 +34050,13 @@
       <x:c r="AT231" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU231" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="232" spans="1:46">
+    <x:row r="232" spans="1:47">
       <x:c r="A232" s="3" t="s">
-        <x:v>275</x:v>
+        <x:v>276</x:v>
       </x:c>
       <x:c r="B232" s="4" t="n">
         <x:v>0</x:v>
@@ -33503,10 +34193,13 @@
       <x:c r="AT232" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU232" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="233" spans="1:46">
+    <x:row r="233" spans="1:47">
       <x:c r="A233" s="3" t="s">
-        <x:v>276</x:v>
+        <x:v>277</x:v>
       </x:c>
       <x:c r="B233" s="4" t="n">
         <x:v>10</x:v>
@@ -33643,10 +34336,13 @@
       <x:c r="AT233" s="4" t="n">
         <x:v>5</x:v>
       </x:c>
+      <x:c r="AU233" s="4" t="n">
+        <x:v>15</x:v>
+      </x:c>
     </x:row>
-    <x:row r="234" spans="1:46">
+    <x:row r="234" spans="1:47">
       <x:c r="A234" s="3" t="s">
-        <x:v>277</x:v>
+        <x:v>278</x:v>
       </x:c>
       <x:c r="B234" s="4" t="n">
         <x:v>0</x:v>
@@ -33783,10 +34479,13 @@
       <x:c r="AT234" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU234" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="235" spans="1:46">
+    <x:row r="235" spans="1:47">
       <x:c r="A235" s="3" t="s">
-        <x:v>278</x:v>
+        <x:v>279</x:v>
       </x:c>
       <x:c r="B235" s="4" t="n">
         <x:v>0</x:v>
@@ -33923,10 +34622,13 @@
       <x:c r="AT235" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU235" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="236" spans="1:46">
+    <x:row r="236" spans="1:47">
       <x:c r="A236" s="3" t="s">
-        <x:v>279</x:v>
+        <x:v>280</x:v>
       </x:c>
       <x:c r="B236" s="4" t="n">
         <x:v>0</x:v>
@@ -34063,10 +34765,13 @@
       <x:c r="AT236" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU236" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="237" spans="1:46">
+    <x:row r="237" spans="1:47">
       <x:c r="A237" s="3" t="s">
-        <x:v>280</x:v>
+        <x:v>281</x:v>
       </x:c>
       <x:c r="B237" s="4" t="n">
         <x:v>0</x:v>
@@ -34203,10 +34908,13 @@
       <x:c r="AT237" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU237" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="238" spans="1:46">
+    <x:row r="238" spans="1:47">
       <x:c r="A238" s="3" t="s">
-        <x:v>281</x:v>
+        <x:v>282</x:v>
       </x:c>
       <x:c r="B238" s="4" t="n">
         <x:v>0</x:v>
@@ -34343,10 +35051,13 @@
       <x:c r="AT238" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU238" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="239" spans="1:46">
+    <x:row r="239" spans="1:47">
       <x:c r="A239" s="3" t="s">
-        <x:v>282</x:v>
+        <x:v>283</x:v>
       </x:c>
       <x:c r="B239" s="4" t="n">
         <x:v>0</x:v>
@@ -34483,10 +35194,13 @@
       <x:c r="AT239" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU239" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="240" spans="1:46">
+    <x:row r="240" spans="1:47">
       <x:c r="A240" s="3" t="s">
-        <x:v>283</x:v>
+        <x:v>284</x:v>
       </x:c>
       <x:c r="B240" s="4" t="n">
         <x:v>0</x:v>
@@ -34623,10 +35337,13 @@
       <x:c r="AT240" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU240" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="241" spans="1:46">
+    <x:row r="241" spans="1:47">
       <x:c r="A241" s="3" t="s">
-        <x:v>284</x:v>
+        <x:v>285</x:v>
       </x:c>
       <x:c r="B241" s="4" t="n">
         <x:v>0</x:v>
@@ -34763,10 +35480,13 @@
       <x:c r="AT241" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU241" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="242" spans="1:46">
+    <x:row r="242" spans="1:47">
       <x:c r="A242" s="3" t="s">
-        <x:v>285</x:v>
+        <x:v>286</x:v>
       </x:c>
       <x:c r="B242" s="4" t="n">
         <x:v>232</x:v>
@@ -34903,10 +35623,13 @@
       <x:c r="AT242" s="4" t="n">
         <x:v>147</x:v>
       </x:c>
+      <x:c r="AU242" s="4" t="n">
+        <x:v>255</x:v>
+      </x:c>
     </x:row>
-    <x:row r="243" spans="1:46">
+    <x:row r="243" spans="1:47">
       <x:c r="A243" s="3" t="s">
-        <x:v>286</x:v>
+        <x:v>287</x:v>
       </x:c>
       <x:c r="B243" s="4" t="n">
         <x:v>51</x:v>
@@ -35043,10 +35766,13 @@
       <x:c r="AT243" s="4" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AU243" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="245" spans="1:46">
+    <x:row r="245" spans="1:47">
       <x:c r="A245" s="5" t="s">
-        <x:v>287</x:v>
+        <x:v>288</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>